<commit_message>
Implement persistent disk for ChromaDB in rag_core.py
</commit_message>
<xml_diff>
--- a/my_documents/BP_Readings.xlsx
+++ b/my_documents/BP_Readings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRED\RAG-PROJECTS\PHLQUERY\my_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4ACBE40-9ED1-4C23-A6CD-CCE89E8E6D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9D07CA-7424-4BB2-B2D8-32D794CF98E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{911A9C29-9135-456E-9569-F6D815BDA784}"/>
+    <workbookView minimized="1" xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{911A9C29-9135-456E-9569-F6D815BDA784}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -118,6 +118,132 @@
   </si>
   <si>
     <t>4:51AM</t>
+  </si>
+  <si>
+    <t>123/76</t>
+  </si>
+  <si>
+    <t>6:51PM</t>
+  </si>
+  <si>
+    <t>06/05/25</t>
+  </si>
+  <si>
+    <t>132/85</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>5:00AM</t>
+  </si>
+  <si>
+    <t>06/06/25</t>
+  </si>
+  <si>
+    <t>132/82</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>136/89</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>5:00PM</t>
+  </si>
+  <si>
+    <t>06/07/25</t>
+  </si>
+  <si>
+    <t>138/89</t>
+  </si>
+  <si>
+    <t>4:46AM</t>
+  </si>
+  <si>
+    <t>133/83</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>5:40PM</t>
+  </si>
+  <si>
+    <t>06/08/25</t>
+  </si>
+  <si>
+    <t>136/85</t>
+  </si>
+  <si>
+    <t>5:37AM</t>
+  </si>
+  <si>
+    <t>06/09/25</t>
+  </si>
+  <si>
+    <t>130/86</t>
+  </si>
+  <si>
+    <t>4:50AM</t>
+  </si>
+  <si>
+    <t>133/87</t>
+  </si>
+  <si>
+    <t>8:24PM</t>
+  </si>
+  <si>
+    <t>06/10/25</t>
+  </si>
+  <si>
+    <t>137/89</t>
+  </si>
+  <si>
+    <t>5:30AM</t>
+  </si>
+  <si>
+    <t>126/76</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>5:55PM</t>
+  </si>
+  <si>
+    <t>06/11/25</t>
+  </si>
+  <si>
+    <t>139/86</t>
+  </si>
+  <si>
+    <t>5:12AM</t>
+  </si>
+  <si>
+    <t>134/88</t>
+  </si>
+  <si>
+    <t>6:23PM</t>
+  </si>
+  <si>
+    <t>06/12/25</t>
+  </si>
+  <si>
+    <t>137/85</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>6:33PM</t>
+  </si>
+  <si>
+    <t>GGNN,..</t>
   </si>
 </sst>
 </file>
@@ -477,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E464AA-B450-41DF-ACD5-7B23E10B225E}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,6 +724,219 @@
         <v>27</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>